<commit_message>
fixed changes on contact forms and app settings
</commit_message>
<xml_diff>
--- a/forms/contact/household-edit.xlsx
+++ b/forms/contact/household-edit.xlsx
@@ -213,7 +213,7 @@
     <t xml:space="preserve">Edit House Hold</t>
   </si>
   <si>
-    <t xml:space="preserve">household_edit</t>
+    <t xml:space="preserve">contact:household:edit</t>
   </si>
   <si>
     <t xml:space="preserve">data</t>
@@ -23033,7 +23033,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10"/>
@@ -24152,7 +24152,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.29296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24218,7 +24218,7 @@
       </c>
       <c r="C2" s="23" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2024-09-03  13-15</v>
+        <v>2024-09-22  11-34</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">

</xml_diff>